<commit_message>
maj commande Mouser après vérifs Bron
</commit_message>
<xml_diff>
--- a/EL_Electrical/Commande-février.xlsx
+++ b/EL_Electrical/Commande-février.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RS Component" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
   <si>
     <t>Description</t>
   </si>
@@ -112,66 +112,6 @@
     <t>Cavity plug</t>
   </si>
   <si>
-    <t>829-12084201</t>
-  </si>
-  <si>
-    <t>Connecteur 0.35-0.50 mm2</t>
-  </si>
-  <si>
-    <t>829-12077411</t>
-  </si>
-  <si>
-    <t>Connecteur 0.50-1.00 mm2</t>
-  </si>
-  <si>
-    <t>829-15363933</t>
-  </si>
-  <si>
-    <t>Connecteur 1.00-2.00 mm2</t>
-  </si>
-  <si>
-    <t>829-12129493</t>
-  </si>
-  <si>
-    <t>Connecteur 2.00-3.00 mm2</t>
-  </si>
-  <si>
-    <t>829-12077413</t>
-  </si>
-  <si>
-    <t>Connecteur 5.00 mm2</t>
-  </si>
-  <si>
-    <t>829-15324983</t>
-  </si>
-  <si>
-    <t>CABLE SEAL DARK RED</t>
-  </si>
-  <si>
-    <t>829-15324985</t>
-  </si>
-  <si>
-    <t>CABLE SEAL PURPLE</t>
-  </si>
-  <si>
-    <t>829-15324982</t>
-  </si>
-  <si>
-    <t>CBL SEAL GREEN</t>
-  </si>
-  <si>
-    <t>829-15324980</t>
-  </si>
-  <si>
-    <t>CBL SEAL GRAY</t>
-  </si>
-  <si>
-    <t>829-15324981</t>
-  </si>
-  <si>
-    <t>CBL SEAL BLUE</t>
-  </si>
-  <si>
     <t>893-3011ASR112VDC</t>
   </si>
   <si>
@@ -266,6 +206,33 @@
   </si>
   <si>
     <t>39-01-2240</t>
+  </si>
+  <si>
+    <t>Coupe-circuit 6 pôles à clef FIA 100A</t>
+  </si>
+  <si>
+    <t>Master switch</t>
+  </si>
+  <si>
+    <t>3110C</t>
+  </si>
+  <si>
+    <t>VIS BANJO SIMPLE AVEC FEU CONTACTEUR DE FEU STOP</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
+  </si>
+  <si>
+    <t>1 en rab celui de l'an dernier avait pété</t>
+  </si>
+  <si>
+    <t>BL99231C</t>
+  </si>
+  <si>
+    <t>Oreca</t>
+  </si>
+  <si>
+    <t>prise booster</t>
   </si>
 </sst>
 </file>
@@ -278,7 +245,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.000\ &quot;€&quot;"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-40C];[Red]\-#,##0.00\ [$€-40C]"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,13 +296,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -347,6 +307,25 @@
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -376,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -428,19 +407,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
       <top style="thin">
         <color theme="1"/>
       </top>
@@ -538,6 +504,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -545,7 +531,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -560,15 +546,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -578,15 +558,11 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -594,31 +570,25 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -643,7 +613,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -889,8 +878,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:I3" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A1:I3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:I11" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:I11"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Composant/Pièce"/>
     <tableColumn id="2" name="Description"/>
@@ -902,7 +891,7 @@
       <calculatedColumnFormula>479/1.2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Lien"/>
-    <tableColumn id="9" name="Colonne1"/>
+    <tableColumn id="9" name="Commentaire"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1173,7 +1162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1221,31 +1210,31 @@
     </row>
     <row r="2" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>57</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>37</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="33">
+      <c r="G2" s="27">
         <v>1.45</v>
       </c>
-      <c r="H2" s="34" t="s">
-        <v>61</v>
+      <c r="H2" s="28" t="s">
+        <v>41</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1257,26 +1246,26 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="7">
         <v>5.66</v>
       </c>
-      <c r="H3" s="34" t="s">
-        <v>65</v>
+      <c r="H3" s="28" t="s">
+        <v>45</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="1"/>
@@ -1289,26 +1278,26 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <v>5.03</v>
       </c>
-      <c r="H4" s="34" t="s">
-        <v>68</v>
+      <c r="H4" s="28" t="s">
+        <v>48</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="1"/>
@@ -1321,28 +1310,28 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="H5" s="34" t="s">
-        <v>69</v>
+      <c r="H5" s="28" t="s">
+        <v>49</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="1"/>
@@ -1355,29 +1344,29 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="F6" s="2">
         <v>5</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <f>1.048*5</f>
         <v>5.24</v>
       </c>
-      <c r="H6" s="34" t="s">
-        <v>77</v>
+      <c r="H6" s="28" t="s">
+        <v>57</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="1"/>
@@ -1395,7 +1384,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="9"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="1"/>
@@ -1413,7 +1402,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="1"/>
@@ -1431,7 +1420,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="9"/>
+      <c r="G9" s="7"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="1"/>
@@ -1449,7 +1438,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="9"/>
+      <c r="G10" s="7"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="1"/>
@@ -1467,7 +1456,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="1"/>
@@ -1485,7 +1474,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="9"/>
+      <c r="G12" s="7"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="1"/>
@@ -1503,7 +1492,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="9"/>
+      <c r="G13" s="7"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="1"/>
@@ -1521,7 +1510,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="9"/>
+      <c r="G14" s="7"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="1"/>
@@ -1539,7 +1528,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="9"/>
+      <c r="G15" s="7"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="1"/>
@@ -1557,7 +1546,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="9"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="1"/>
@@ -1575,7 +1564,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="9"/>
+      <c r="G17" s="7"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="1"/>
@@ -1593,7 +1582,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="9"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="1"/>
@@ -1611,7 +1600,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="9"/>
+      <c r="G19" s="7"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="1"/>
@@ -1630,8 +1619,8 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1658,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,512 +1661,232 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="20" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="27" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="23">
         <v>21.23</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="23">
         <f>1.2*D2</f>
         <v>25.475999999999999</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="27">
+      <c r="F2" s="22"/>
+      <c r="G2" s="21">
         <v>1</v>
       </c>
-      <c r="H2" s="29">
+      <c r="H2" s="23">
         <f>D2*G2</f>
         <v>21.23</v>
       </c>
-      <c r="I2" s="29">
+      <c r="I2" s="23">
         <f>E2*G2</f>
         <v>25.475999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="23">
         <v>0.19</v>
       </c>
-      <c r="E3" s="29">
-        <f t="shared" ref="E3:E17" si="0">1.2*D3</f>
+      <c r="E3" s="23">
+        <f t="shared" ref="E3:E7" si="0">1.2*D3</f>
         <v>0.22799999999999998</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="27">
+      <c r="F3" s="22"/>
+      <c r="G3" s="21">
         <v>30</v>
       </c>
-      <c r="H3" s="29">
-        <f t="shared" ref="H3:H17" si="1">D3*G3</f>
+      <c r="H3" s="23">
+        <f t="shared" ref="H3:H7" si="1">D3*G3</f>
         <v>5.7</v>
       </c>
-      <c r="I3" s="29">
-        <f t="shared" ref="I3:I17" si="2">E3*G3</f>
+      <c r="I3" s="23">
+        <f t="shared" ref="I3:I7" si="2">E3*G3</f>
         <v>6.84</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="29">
-        <v>0.22</v>
-      </c>
-      <c r="E4" s="29">
-        <f t="shared" si="0"/>
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="27">
-        <v>25</v>
-      </c>
-      <c r="H4" s="29">
-        <f t="shared" si="1"/>
-        <v>5.5</v>
-      </c>
-      <c r="I4" s="29">
-        <f t="shared" si="2"/>
-        <v>6.6000000000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="29">
-        <v>0.39</v>
-      </c>
-      <c r="E5" s="29">
-        <f t="shared" si="0"/>
-        <v>0.46799999999999997</v>
-      </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="27">
-        <v>25</v>
-      </c>
-      <c r="H5" s="29">
-        <f t="shared" si="1"/>
-        <v>9.75</v>
-      </c>
-      <c r="I5" s="29">
-        <f t="shared" si="2"/>
-        <v>11.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="29">
-        <v>0.22</v>
-      </c>
-      <c r="E6" s="29">
-        <f t="shared" si="0"/>
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="27">
-        <v>25</v>
-      </c>
-      <c r="H6" s="29">
-        <f t="shared" si="1"/>
-        <v>5.5</v>
-      </c>
-      <c r="I6" s="29">
-        <f t="shared" si="2"/>
-        <v>6.6000000000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="29">
-        <v>0.24</v>
-      </c>
-      <c r="E7" s="29">
-        <f t="shared" si="0"/>
-        <v>0.28799999999999998</v>
-      </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="27">
-        <v>25</v>
-      </c>
-      <c r="H7" s="29">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="I7" s="29">
-        <f t="shared" si="2"/>
-        <v>7.1999999999999993</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="29">
-        <v>0.23</v>
-      </c>
-      <c r="E8" s="29">
-        <f t="shared" si="0"/>
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="27">
-        <v>25</v>
-      </c>
-      <c r="H8" s="29">
-        <f t="shared" si="1"/>
-        <v>5.75</v>
-      </c>
-      <c r="I8" s="29">
-        <f t="shared" si="2"/>
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="29">
-        <v>0.13</v>
-      </c>
-      <c r="E9" s="29">
-        <f t="shared" si="0"/>
-        <v>0.156</v>
-      </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="27">
-        <v>25</v>
-      </c>
-      <c r="H9" s="29">
-        <f t="shared" si="1"/>
-        <v>3.25</v>
-      </c>
-      <c r="I9" s="29">
-        <f t="shared" si="2"/>
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29">
-        <v>0.08</v>
-      </c>
-      <c r="E10" s="29">
-        <f t="shared" si="0"/>
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="27">
-        <v>25</v>
-      </c>
-      <c r="H10" s="29">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I10" s="29">
-        <f t="shared" si="2"/>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29">
-        <v>0.1</v>
-      </c>
-      <c r="E11" s="29">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
-      </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="27">
-        <v>25</v>
-      </c>
-      <c r="H11" s="29">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="I11" s="29">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29">
-        <v>0.1</v>
-      </c>
-      <c r="E12" s="29">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
-      </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="27">
-        <v>25</v>
-      </c>
-      <c r="H12" s="29">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="I12" s="29">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="29">
-        <v>0.1</v>
-      </c>
-      <c r="E13" s="29">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
-      </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="27">
-        <v>25</v>
-      </c>
-      <c r="H13" s="29">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="I13" s="29">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="29">
+      <c r="D4" s="23">
         <v>3.19</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E4" s="23">
         <f t="shared" si="0"/>
         <v>3.8279999999999998</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="27">
+      <c r="F4" s="22"/>
+      <c r="G4" s="21">
         <v>4</v>
       </c>
-      <c r="H14" s="29">
+      <c r="H4" s="23">
         <f t="shared" si="1"/>
         <v>12.76</v>
       </c>
-      <c r="I14" s="29">
+      <c r="I4" s="23">
         <f t="shared" si="2"/>
         <v>15.311999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="27" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D5" s="23">
         <v>46.31</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E5" s="23">
         <f t="shared" si="0"/>
         <v>55.572000000000003</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="27">
+      <c r="F5" s="22"/>
+      <c r="G5" s="21">
         <v>1</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H5" s="23">
         <f t="shared" si="1"/>
         <v>46.31</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I5" s="23">
         <f t="shared" si="2"/>
         <v>55.572000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="29">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="23">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E6" s="23">
         <f t="shared" si="0"/>
         <v>5.28</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="27">
+      <c r="F6" s="22"/>
+      <c r="G6" s="21">
         <v>1</v>
       </c>
-      <c r="H16" s="29">
+      <c r="H6" s="23">
         <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="I16" s="29">
+      <c r="I6" s="23">
         <f t="shared" si="2"/>
         <v>5.28</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="29">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="23">
         <v>4.8600000000000003</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E7" s="23">
         <f t="shared" si="0"/>
         <v>5.8319999999999999</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="27">
+      <c r="F7" s="22"/>
+      <c r="G7" s="21">
         <v>1</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H7" s="23">
         <f t="shared" si="1"/>
         <v>4.8600000000000003</v>
       </c>
-      <c r="I17" s="29">
+      <c r="I7" s="23">
         <f t="shared" si="2"/>
         <v>5.8319999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G18" s="30"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="36">
-        <f>SUM(I2:I17)</f>
-        <v>168.61199999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="39">
+        <f>SUM(I2:I7)</f>
+        <v>114.312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D19:H20"/>
-    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="D9:H10"/>
+    <mergeCell ref="I9:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2185,96 +1894,217 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="8" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="38.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="I1" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="9">
         <v>1</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="10">
         <f t="shared" ref="G2" si="0">479/1.2</f>
         <v>399.16666666666669</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="14" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="15"/>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31">
+        <v>1</v>
+      </c>
+      <c r="G3" s="33">
+        <v>15.95</v>
+      </c>
+      <c r="H3" s="34"/>
+    </row>
+    <row r="4" spans="1:9" ht="45.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="31">
+        <v>2</v>
+      </c>
+      <c r="G4" s="36">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="H4" s="22"/>
+      <c r="I4" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22">
+        <v>6331</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="31">
+        <v>1</v>
+      </c>
+      <c r="G5" s="36">
+        <v>9.9</v>
+      </c>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout antenne GPS aux commandes
</commit_message>
<xml_diff>
--- a/EL_Electrical/Commande-février.xlsx
+++ b/EL_Electrical/Commande-février.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="RS Component" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
   <si>
     <t>Description</t>
   </si>
@@ -233,6 +233,24 @@
   </si>
   <si>
     <t>prise booster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antenne GPS </t>
+  </si>
+  <si>
+    <t>plus petit fil (50cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">140-8050 </t>
+  </si>
+  <si>
+    <t>Siretta</t>
+  </si>
+  <si>
+    <t>MIKE3A/0.5M/SMAM/RA/S/17</t>
+  </si>
+  <si>
+    <t>https://fr.rs-online.com/web/p/antennes-gps/1408050/</t>
   </si>
 </sst>
 </file>
@@ -1162,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,14 +1396,30 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>74</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1636,11 +1670,12 @@
     <hyperlink ref="H4" r:id="rId2"/>
     <hyperlink ref="H5" r:id="rId3"/>
     <hyperlink ref="H6" r:id="rId4"/>
+    <hyperlink ref="H7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1649,7 +1684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>